<commit_message>
added support for "special" veins that use their own blocks instead of gt's ores, added anthractite and sylvite
</commit_message>
<xml_diff>
--- a/OresToFieldGuide/data/sheet.xlsx
+++ b/OresToFieldGuide/data/sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="423">
   <si>
     <t>Vein ID</t>
   </si>
@@ -961,6 +961,12 @@
     <t>dripstone</t>
   </si>
   <si>
+    <t>nether_anthracite</t>
+  </si>
+  <si>
+    <t>anthracite: 100</t>
+  </si>
+  <si>
     <t>nether_apatite</t>
   </si>
   <si>
@@ -1259,6 +1265,12 @@
   </si>
   <si>
     <t>sphalerite: 15 [1]</t>
+  </si>
+  <si>
+    <t>nether_sylvite</t>
+  </si>
+  <si>
+    <t>sylvite: 100</t>
   </si>
   <si>
     <t>nether_tetrahedrite</t>
@@ -1376,7 +1388,9 @@
     <col min="38" max="38" width="9.140625" customWidth="1" style="1"/>
     <col min="39" max="39" width="9.140625" customWidth="1" style="1"/>
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
-    <col min="41" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
+    <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -6045,7 +6059,9 @@
     <col min="38" max="38" width="9.140625" customWidth="1" style="1"/>
     <col min="39" max="39" width="9.140625" customWidth="1" style="1"/>
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
-    <col min="41" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
+    <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -7143,7 +7159,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" state="frozen" activePane="bottomLeft"/>
@@ -7192,7 +7208,9 @@
     <col min="38" max="38" width="9.140625" customWidth="1" style="1"/>
     <col min="39" max="39" width="9.140625" customWidth="1" style="1"/>
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
-    <col min="41" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
+    <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -7259,32 +7277,29 @@
         <v>315</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
-        <v>0.35</v>
+        <v>0.8</v>
       </c>
       <c r="E2" s="1">
         <v>48</v>
       </c>
       <c r="F2" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G2" s="1">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="O2" s="1" t="s">
         <v>36</v>
       </c>
@@ -7292,7 +7307,7 @@
         <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>36</v>
@@ -7304,27 +7319,27 @@
         <v>36</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="E3" s="1">
         <v>48</v>
@@ -7333,25 +7348,19 @@
         <v>128</v>
       </c>
       <c r="G3" s="1">
-        <v>48</v>
-      </c>
-      <c r="H3" s="1">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>36</v>
@@ -7369,60 +7378,66 @@
         <v>36</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1">
         <v>0.4</v>
       </c>
       <c r="E4" s="1">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1">
         <v>128</v>
       </c>
       <c r="G4" s="1">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>325</v>
+      <c r="M4" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>36</v>
@@ -7431,7 +7446,7 @@
         <v>36</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>36</v>
@@ -7439,16 +7454,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="D5" s="1">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="E5" s="1">
         <v>32</v>
@@ -7456,20 +7471,17 @@
       <c r="F5" s="1">
         <v>128</v>
       </c>
-      <c r="H5" s="1">
-        <v>60</v>
-      </c>
-      <c r="I5" s="1">
-        <v>12</v>
+      <c r="G5" s="1">
+        <v>45</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>252</v>
+        <v>325</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>253</v>
+        <v>326</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>107</v>
+        <v>327</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>37</v>
@@ -7501,16 +7513,16 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="D6" s="1">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="E6" s="1">
         <v>32</v>
@@ -7518,46 +7530,52 @@
       <c r="F6" s="1">
         <v>128</v>
       </c>
-      <c r="G6" s="1">
-        <v>45</v>
+      <c r="H6" s="1">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1">
+        <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>328</v>
+        <v>252</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>329</v>
+        <v>253</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
@@ -7578,60 +7596,54 @@
         <v>45</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="O7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="D8" s="1">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
         <v>128</v>
@@ -7639,20 +7651,17 @@
       <c r="G8" s="1">
         <v>45</v>
       </c>
-      <c r="H8" s="1">
-        <v>8</v>
-      </c>
       <c r="J8" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>37</v>
@@ -7684,19 +7693,19 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="D9" s="1">
         <v>0.35</v>
       </c>
       <c r="E9" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
         <v>128</v>
@@ -7704,20 +7713,23 @@
       <c r="G9" s="1">
         <v>45</v>
       </c>
+      <c r="H9" s="1">
+        <v>8</v>
+      </c>
       <c r="J9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>37</v>
@@ -7726,39 +7738,39 @@
         <v>37</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="1">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="D10" s="1">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="E10" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>128</v>
@@ -7767,19 +7779,16 @@
         <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>128</v>
+        <v>341</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>129</v>
+        <v>342</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>343</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>36</v>
@@ -7788,25 +7797,25 @@
         <v>37</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
@@ -7817,49 +7826,52 @@
         <v>42</v>
       </c>
       <c r="C11" s="1">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="D11" s="1">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F11" s="1">
         <v>128</v>
       </c>
       <c r="G11" s="1">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>56</v>
+        <v>274</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>36</v>
@@ -7873,16 +7885,16 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="1">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="D12" s="1">
-        <v>0.55</v>
+        <v>0.45</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -7894,57 +7906,57 @@
         <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>43</v>
+        <v>347</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>44</v>
+        <v>348</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="D13" s="1">
-        <v>0.35</v>
+        <v>0.55</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -7952,20 +7964,20 @@
       <c r="F13" s="1">
         <v>128</v>
       </c>
-      <c r="H13" s="1">
-        <v>60</v>
-      </c>
-      <c r="I13" s="1">
-        <v>12</v>
+      <c r="G13" s="1">
+        <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>349</v>
+        <v>43</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>350</v>
+        <v>44</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>351</v>
+        <v>45</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>36</v>
@@ -7997,16 +8009,16 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -8014,50 +8026,47 @@
       <c r="F14" s="1">
         <v>128</v>
       </c>
-      <c r="G14" s="1">
-        <v>35</v>
+      <c r="H14" s="1">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1">
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>48</v>
+        <v>351</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>49</v>
+        <v>352</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="O14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
@@ -8071,31 +8080,34 @@
         <v>220</v>
       </c>
       <c r="D15" s="1">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="E15" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <v>128</v>
       </c>
       <c r="G15" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="M15" s="1" t="s">
-        <v>149</v>
+        <v>51</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>37</v>
@@ -8124,13 +8136,13 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D16" s="1">
         <v>0.35</v>
@@ -8142,22 +8154,19 @@
         <v>128</v>
       </c>
       <c r="G16" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="M16" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>36</v>
@@ -8166,125 +8175,128 @@
         <v>37</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="1">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="D17" s="1">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1">
         <v>128</v>
       </c>
       <c r="G17" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>58</v>
+        <v>361</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="N17" s="1" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="1">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D18" s="1">
         <v>0.4</v>
       </c>
       <c r="E18" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <v>128</v>
       </c>
       <c r="G18" s="1">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>168</v>
+      <c r="N18" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>37</v>
@@ -8316,16 +8328,16 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="1">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="D19" s="1">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E19" s="1">
         <v>32</v>
@@ -8334,81 +8346,81 @@
         <v>128</v>
       </c>
       <c r="G19" s="1">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>279</v>
+        <v>370</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="M19" s="1" t="s">
-        <v>374</v>
+        <v>168</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="1">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="D20" s="1">
-        <v>0.55</v>
+        <v>0.35</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1">
         <v>128</v>
       </c>
       <c r="G20" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>64</v>
+        <v>279</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>65</v>
+        <v>374</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>66</v>
+        <v>375</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>67</v>
+        <v>376</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>36</v>
@@ -8440,34 +8452,37 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="1">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="D21" s="1">
-        <v>0.35</v>
+        <v>0.55</v>
       </c>
       <c r="E21" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
         <v>128</v>
       </c>
       <c r="G21" s="1">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>377</v>
+        <v>64</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>378</v>
+        <v>65</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>379</v>
+        <v>66</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>36</v>
@@ -8499,34 +8514,37 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="1">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="D22" s="1">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="G22" s="1">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="O22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>37</v>
@@ -8535,27 +8553,27 @@
         <v>36</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>42</v>
@@ -8564,29 +8582,23 @@
         <v>250</v>
       </c>
       <c r="D23" s="1">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E23" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="G23" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="O23" s="1" t="s">
         <v>37</v>
       </c>
@@ -8594,13 +8606,13 @@
         <v>37</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>36</v>
@@ -8617,72 +8629,78 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="1">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="D24" s="1">
-        <v>0.55</v>
+        <v>0.35</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1">
         <v>128</v>
       </c>
       <c r="G24" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>69</v>
+        <v>386</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>70</v>
+        <v>387</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="1">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="D25" s="1">
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -8691,57 +8709,54 @@
         <v>128</v>
       </c>
       <c r="G25" s="1">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>389</v>
+        <v>69</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>188</v>
+        <v>70</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="1">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -8753,31 +8768,31 @@
         <v>45</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>190</v>
+        <v>391</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>392</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>393</v>
+        <v>188</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>36</v>
@@ -8791,38 +8806,35 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="1">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="D27" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
         <v>128</v>
       </c>
       <c r="G27" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>297</v>
+        <v>190</v>
       </c>
       <c r="K27" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="O27" s="1" t="s">
         <v>36</v>
       </c>
@@ -8833,60 +8845,57 @@
         <v>36</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>37</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="D28" s="1">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F28" s="1">
         <v>128</v>
       </c>
       <c r="G28" s="1">
-        <v>33</v>
-      </c>
-      <c r="H28" s="1">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>72</v>
+        <v>297</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>73</v>
+        <v>397</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>398</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>399</v>
+        <v>202</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>36</v>
@@ -8918,10 +8927,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1">
         <v>180</v>
@@ -8936,16 +8945,22 @@
         <v>128</v>
       </c>
       <c r="G29" s="1">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="H29" s="1">
+        <v>8</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>402</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>36</v>
@@ -8977,16 +8992,16 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="1">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="D30" s="1">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -8995,102 +9010,102 @@
         <v>128</v>
       </c>
       <c r="G30" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>81</v>
+        <v>403</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>84</v>
+        <v>404</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="1">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="D31" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E31" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
         <v>128</v>
       </c>
       <c r="G31" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>405</v>
+        <v>81</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>406</v>
+        <v>82</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>407</v>
+        <v>83</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>36</v>
@@ -9098,19 +9113,19 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="1">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D32" s="1">
         <v>0.5</v>
       </c>
       <c r="E32" s="1">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F32" s="1">
         <v>128</v>
@@ -9119,37 +9134,37 @@
         <v>45</v>
       </c>
       <c r="J32" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="O32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>36</v>
@@ -9157,35 +9172,35 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="1">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D33" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F33" s="1">
         <v>128</v>
       </c>
       <c r="G33" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J33" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>414</v>
-      </c>
       <c r="O33" s="1" t="s">
         <v>37</v>
       </c>
@@ -9193,13 +9208,13 @@
         <v>37</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T33" s="1" t="s">
         <v>36</v>
@@ -9211,60 +9226,60 @@
         <v>36</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="1">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D34" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="E34" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1">
         <v>128</v>
       </c>
       <c r="G34" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="O34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>36</v>
@@ -9275,66 +9290,178 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1">
-        <v>180</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
+        <v>64</v>
+      </c>
+      <c r="G35" s="1">
+        <v>17</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="1">
+        <v>170</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>32</v>
+      </c>
+      <c r="F36" s="1">
         <v>128</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G36" s="1">
+        <v>45</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1">
+        <v>180</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>128</v>
+      </c>
+      <c r="G37" s="1">
         <v>33</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H37" s="1">
         <v>7</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W35" s="1" t="s">
+      <c r="O37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W37" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix icon in field guide for moon veins
</commit_message>
<xml_diff>
--- a/OresToFieldGuide/data/sheet.xlsx
+++ b/OresToFieldGuide/data/sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
   <si>
     <t>Vein ID</t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>copper: 20</t>
+  </si>
+  <si>
+    <t>glacio_stone</t>
   </si>
   <si>
     <t>moon_deepslate</t>
@@ -1390,7 +1393,8 @@
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
     <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
     <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
-    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="43" width="9.140625" customWidth="1" style="1"/>
+    <col min="44" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -6010,7 +6014,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" state="frozen" activePane="bottomLeft"/>
@@ -6036,11 +6040,11 @@
     <col min="15" max="15" width="9.140625" customWidth="1" style="1"/>
     <col min="16" max="16" width="9.140625" customWidth="1" style="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1" style="1"/>
-    <col min="18" max="18" width="16.501888275146484" customWidth="1" style="1"/>
-    <col min="19" max="19" width="12.735984802246094" customWidth="1" style="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1" style="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1" style="1"/>
-    <col min="22" max="22" width="9.140625" customWidth="1" style="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1" style="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1" style="1"/>
+    <col min="20" max="20" width="12.71347713470459" customWidth="1" style="1"/>
+    <col min="21" max="21" width="16.501888275146484" customWidth="1" style="1"/>
+    <col min="22" max="22" width="12.735984802246094" customWidth="1" style="1"/>
     <col min="23" max="23" width="9.140625" customWidth="1" style="1"/>
     <col min="24" max="24" width="9.140625" customWidth="1" style="1"/>
     <col min="25" max="25" width="9.140625" customWidth="1" style="1"/>
@@ -6061,7 +6065,8 @@
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
     <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
     <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
-    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="43" width="9.140625" customWidth="1" style="1"/>
+    <col min="44" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -6096,24 +6101,36 @@
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>243</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>42</v>
@@ -6134,19 +6151,19 @@
         <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>36</v>
@@ -6155,12 +6172,24 @@
         <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>42</v>
@@ -6181,36 +6210,48 @@
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>102</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>104</v>
@@ -6234,33 +6275,45 @@
         <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>107</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>42</v>
@@ -6281,16 +6334,16 @@
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>36</v>
@@ -6302,15 +6355,27 @@
         <v>36</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>42</v>
@@ -6331,36 +6396,48 @@
         <v>36</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
@@ -6381,36 +6458,48 @@
         <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -6431,36 +6520,48 @@
         <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>157</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>42</v>
@@ -6490,7 +6591,7 @@
         <v>130</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>132</v>
@@ -6499,21 +6600,33 @@
         <v>36</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>42</v>
@@ -6534,13 +6647,13 @@
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>59</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>61</v>
@@ -6552,21 +6665,33 @@
         <v>36</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>42</v>
@@ -6587,7 +6712,7 @@
         <v>25</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>171</v>
@@ -6602,21 +6727,33 @@
         <v>36</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>42</v>
@@ -6649,24 +6786,36 @@
         <v>67</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>42</v>
@@ -6687,7 +6836,7 @@
         <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>176</v>
@@ -6699,21 +6848,33 @@
         <v>36</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>42</v>
@@ -6734,36 +6895,48 @@
         <v>40</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>42</v>
@@ -6784,13 +6957,13 @@
         <v>15</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>36</v>
@@ -6802,15 +6975,27 @@
         <v>36</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>42</v>
@@ -6831,16 +7016,16 @@
         <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>37</v>
@@ -6855,12 +7040,24 @@
         <v>37</v>
       </c>
       <c r="S16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -6899,15 +7096,27 @@
         <v>36</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
@@ -6928,22 +7137,22 @@
         <v>35</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>201</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q18" s="1" t="s">
         <v>36</v>
@@ -6952,12 +7161,24 @@
         <v>37</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>31</v>
@@ -6984,7 +7205,7 @@
         <v>72</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>74</v>
@@ -6993,24 +7214,36 @@
         <v>75</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>42</v>
@@ -7031,33 +7264,45 @@
         <v>20</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>42</v>
@@ -7081,33 +7326,45 @@
         <v>81</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>84</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>42</v>
@@ -7131,10 +7388,10 @@
         <v>204</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>36</v>
@@ -7146,10 +7403,22 @@
         <v>36</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7479,8 @@
     <col min="40" max="40" width="9.140625" customWidth="1" style="1"/>
     <col min="41" max="41" width="9.140625" customWidth="1" style="1"/>
     <col min="42" max="42" width="9.140625" customWidth="1" style="1"/>
-    <col min="43" max="16384" width="9.140625" customWidth="1" style="1"/>
+    <col min="43" max="43" width="9.140625" customWidth="1" style="1"/>
+    <col min="44" max="16384" width="9.140625" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1">
@@ -7248,16 +7518,16 @@
         <v>11</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>19</v>
@@ -7274,7 +7544,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
@@ -7298,7 +7568,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>36</v>
@@ -7330,7 +7600,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>42</v>
@@ -7351,10 +7621,10 @@
         <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>93</v>
@@ -7389,7 +7659,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -7413,13 +7683,13 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>98</v>
@@ -7454,7 +7724,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>42</v>
@@ -7475,13 +7745,13 @@
         <v>45</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>37</v>
@@ -7513,7 +7783,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>104</v>
@@ -7537,10 +7807,10 @@
         <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>107</v>
@@ -7575,7 +7845,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
@@ -7596,10 +7866,10 @@
         <v>45</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>36</v>
@@ -7631,7 +7901,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -7652,16 +7922,16 @@
         <v>45</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>119</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>37</v>
@@ -7693,7 +7963,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
@@ -7717,16 +7987,16 @@
         <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>37</v>
@@ -7758,7 +8028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>42</v>
@@ -7779,13 +8049,13 @@
         <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>126</v>
@@ -7820,7 +8090,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>42</v>
@@ -7847,10 +8117,10 @@
         <v>129</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>132</v>
@@ -7885,7 +8155,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>42</v>
@@ -7906,10 +8176,10 @@
         <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>45</v>
@@ -7947,7 +8217,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>42</v>
@@ -8009,7 +8279,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>104</v>
@@ -8033,13 +8303,13 @@
         <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>36</v>
@@ -8071,7 +8341,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>42</v>
@@ -8098,7 +8368,7 @@
         <v>49</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>51</v>
@@ -8136,7 +8406,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>42</v>
@@ -8157,13 +8427,13 @@
         <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>149</v>
@@ -8198,7 +8468,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -8219,16 +8489,16 @@
         <v>41</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>158</v>
@@ -8263,7 +8533,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
@@ -8287,13 +8557,13 @@
         <v>58</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>62</v>
@@ -8328,7 +8598,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>42</v>
@@ -8349,13 +8619,13 @@
         <v>45</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>168</v>
@@ -8390,7 +8660,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>42</v>
@@ -8411,16 +8681,16 @@
         <v>41</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>36</v>
@@ -8452,7 +8722,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>42</v>
@@ -8514,7 +8784,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>42</v>
@@ -8535,13 +8805,13 @@
         <v>45</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>36</v>
@@ -8573,7 +8843,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>42</v>
@@ -8594,10 +8864,10 @@
         <v>32</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>37</v>
@@ -8629,7 +8899,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>42</v>
@@ -8650,13 +8920,13 @@
         <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>184</v>
@@ -8691,7 +8961,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>42</v>
@@ -8747,7 +9017,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>42</v>
@@ -8768,10 +9038,10 @@
         <v>45</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>188</v>
@@ -8806,7 +9076,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>42</v>
@@ -8830,10 +9100,10 @@
         <v>190</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>36</v>
@@ -8865,7 +9135,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>42</v>
@@ -8886,13 +9156,13 @@
         <v>50</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>202</v>
@@ -8927,7 +9197,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
@@ -8957,10 +9227,10 @@
         <v>73</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>36</v>
@@ -8992,7 +9262,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>42</v>
@@ -9013,13 +9283,13 @@
         <v>25</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>36</v>
@@ -9051,7 +9321,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -9113,7 +9383,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
@@ -9134,13 +9404,13 @@
         <v>45</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>36</v>
@@ -9172,7 +9442,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -9193,13 +9463,13 @@
         <v>45</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>209</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>37</v>
@@ -9231,7 +9501,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>42</v>
@@ -9252,13 +9522,13 @@
         <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>37</v>
@@ -9290,7 +9560,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>42</v>
@@ -9311,7 +9581,7 @@
         <v>17</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>36</v>
@@ -9343,7 +9613,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>42</v>
@@ -9364,10 +9634,10 @@
         <v>45</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>222</v>
@@ -9402,7 +9672,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>31</v>

</xml_diff>